<commit_message>
worked on flow controller but struggling with flow controller.
</commit_message>
<xml_diff>
--- a/ErrorDocumentation.xlsx
+++ b/ErrorDocumentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>S.No</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>error:MultipartFile cannot be resolved to a type sol:</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>exception: SQLGrammarException</t>
   </si>
 </sst>
 </file>
@@ -441,15 +447,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="31.33203125" customWidth="1"/>
     <col min="5" max="6" width="35.44140625" customWidth="1"/>
@@ -633,6 +640,24 @@
         <v>29</v>
       </c>
     </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2">
+        <v>42707</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
couldn't resolve that register  error.
</commit_message>
<xml_diff>
--- a/ErrorDocumentation.xlsx
+++ b/ErrorDocumentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>S.No</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>exception: SQLGrammarException</t>
+  </si>
+  <si>
+    <t>Sequence "HIBERNATE_SEQUENCE" not found; SQL statement:</t>
   </si>
 </sst>
 </file>
@@ -447,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,6 +661,11 @@
         <v>31</v>
       </c>
     </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
security done product fetching done showing categories pn menubar done . can navigate to product detail
</commit_message>
<xml_diff>
--- a/ErrorDocumentation.xlsx
+++ b/ErrorDocumentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>S.No</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Sequence "HIBERNATE_SEQUENCE" not found; SQL statement:</t>
+  </si>
+  <si>
+    <t>org.springframework.dao.DataIntegrityViolationException: could not execute statement; SQL [n/a]; constraint ["FK_USERROLE_USER_ID: PUBLIC.USERROLE FOREIGN KEY(USER_ID) REFERENCES PUBLIC.USER(USER_ID) (0)"; SQL statement:</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,7 +665,26 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
       <c r="I12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
worked on cart controller.
</commit_message>
<xml_diff>
--- a/ErrorDocumentation.xlsx
+++ b/ErrorDocumentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>S.No</t>
   </si>
@@ -122,10 +122,22 @@
     <t>exception: SQLGrammarException</t>
   </si>
   <si>
-    <t>Sequence "HIBERNATE_SEQUENCE" not found; SQL statement:</t>
-  </si>
-  <si>
-    <t>org.springframework.dao.DataIntegrityViolationException: could not execute statement; SQL [n/a]; constraint ["FK_USERROLE_USER_ID: PUBLIC.USERROLE FOREIGN KEY(USER_ID) REFERENCES PUBLIC.USER(USER_ID) (0)"; SQL statement:</t>
+    <t>Error creating bean with name 'adminController': Unsatisfied dependency expressed through field 'categoryDAO'</t>
+  </si>
+  <si>
+    <t>Sequence "HIBERNATE_SEQUENCE" not found; SQL statement: sol:made auto generate type as identity</t>
+  </si>
+  <si>
+    <t>org.springframework.dao.DataIntegrityViolationException: could not execute statement; SQL [n/a]; constraint ["FK_USERROLE_USER_ID: PUBLIC.USERROLE FOREIGN KEY(USER_ID) REFERENCES PUBLIC.USER(USER_ID) (0)"; SQL statement: sol: check if field names are proper</t>
+  </si>
+  <si>
+    <t>20m</t>
+  </si>
+  <si>
+    <t>java.io.StreamCorruptedException: invalid type code:</t>
+  </si>
+  <si>
+    <t>java.lang.ClassCastException: cannot assign instance of java.lang.StackTraceElement to field java.util.Collections$UnmodifiableList.list of type java.util.List in instance of java.util.Collections$UnmodifiableList</t>
   </si>
 </sst>
 </file>
@@ -453,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,28 +676,85 @@
         <v>31</v>
       </c>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2">
+        <v>42711</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <v>42711</v>
+      </c>
       <c r="H12" t="s">
         <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2">
+        <v>42711</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
       <c r="H13" t="s">
         <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2">
+        <v>42711</v>
+      </c>
       <c r="H14" t="s">
         <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <v>42711</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <v>42711</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cart in progress. fetching product in cart is done.
</commit_message>
<xml_diff>
--- a/ErrorDocumentation.xlsx
+++ b/ErrorDocumentation.xlsx
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
started working on webflow. webflow initiated.
</commit_message>
<xml_diff>
--- a/ErrorDocumentation.xlsx
+++ b/ErrorDocumentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>S.No</t>
   </si>
@@ -138,6 +138,10 @@
   </si>
   <si>
     <t>java.lang.ClassCastException: cannot assign instance of java.lang.StackTraceElement to field java.util.Collections$UnmodifiableList.list of type java.util.List in instance of java.util.Collections$UnmodifiableList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTP Status 500 - Request processing failed; nested exception is java.lang.IllegalArgumentException: Unable to load class 'com.niit.gauresh_backEnd.model.ShippingAddress'
+</t>
   </si>
 </sst>
 </file>
@@ -181,10 +185,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,6 +764,11 @@
         <v>37</v>
       </c>
     </row>
+    <row r="17" spans="9:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="I17" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>